<commit_message>
Add Outmigration Form feature
</commit_message>
<xml_diff>
--- a/app/src/main/res/raw/outmigration_form.xlsx
+++ b/app/src/main/res/raw/outmigration_form.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="17670" tabRatio="500"/>
+    <workbookView windowWidth="26265" windowHeight="12105" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="columns" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="141">
   <si>
     <t>group</t>
   </si>
@@ -145,7 +145,7 @@
     <t>2.1. Migration Type</t>
   </si>
   <si>
-    <t>2.1. Tipo de Imigração</t>
+    <t>2.1. Tipo de Emigração</t>
   </si>
   <si>
     <t>selected_only</t>
@@ -202,10 +202,10 @@
     <t>reasons</t>
   </si>
   <si>
-    <t>5.2. Reason for In Migration</t>
-  </si>
-  <si>
-    <t>5.2. Causas da migração</t>
+    <t>5.2. Reason for Outmigration</t>
+  </si>
+  <si>
+    <t>5.2. Causas da emigração</t>
   </si>
   <si>
     <t>migrationReasonOther</t>
@@ -214,7 +214,7 @@
     <t>5.2.1. Specify other reason for migration</t>
   </si>
   <si>
-    <t>5.2.1. Especifique outras causas da migração</t>
+    <t>5.2.1. Especifique outras causas da emigração</t>
   </si>
   <si>
     <t>${migrationReason} = 'OTHER'</t>
@@ -367,13 +367,13 @@
     <t>Não sabe</t>
   </si>
   <si>
-    <t>ENT</t>
-  </si>
-  <si>
-    <t>Internal InMigration</t>
-  </si>
-  <si>
-    <t>Imigração Interna</t>
+    <t>EXT</t>
+  </si>
+  <si>
+    <t>External Outmigration</t>
+  </si>
+  <si>
+    <t>Emigração Externa</t>
   </si>
   <si>
     <t>CAME_WITH_RELATIVES</t>
@@ -473,9 +473,6 @@
   </si>
   <si>
     <t>External OutMigration</t>
-  </si>
-  <si>
-    <t>Emigração Externa</t>
   </si>
 </sst>
 </file>
@@ -484,9 +481,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -534,13 +531,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="0"/>
       <name val="Arial"/>
       <charset val="0"/>
@@ -555,6 +545,57 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -564,16 +605,23 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Arial"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -587,38 +635,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -632,47 +665,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -708,31 +705,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -744,139 +873,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -905,6 +902,30 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -923,17 +944,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -967,168 +984,148 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="18" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1489,8 +1486,8 @@
   <sheetPr/>
   <dimension ref="A1:O29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="12.75"/>
@@ -1612,7 +1609,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:13">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
@@ -1631,6 +1628,9 @@
       <c r="J4" s="13"/>
       <c r="K4" s="13"/>
       <c r="L4" t="b">
+        <v>1</v>
+      </c>
+      <c r="M4" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1946,7 +1946,7 @@
   <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D16" sqref="C16:D16"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelCol="4"/>
@@ -2442,7 +2442,7 @@
         <v>140</v>
       </c>
       <c r="C2" t="s">
-        <v>141</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Rename FormMapping Converter to a generic MapString Converter - Add more sync entities and renaming strings.xml
</commit_message>
<xml_diff>
--- a/app/src/main/res/raw/outmigration_form.xlsx
+++ b/app/src/main/res/raw/outmigration_form.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="26265" windowHeight="9390" tabRatio="500"/>
+    <workbookView windowHeight="7350" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="columns" sheetId="1" r:id="rId1"/>
@@ -469,7 +469,7 @@
     <t>form_name::pt</t>
   </si>
   <si>
-    <t>rawInMigration</t>
+    <t>rawOutMigration</t>
   </si>
   <si>
     <t>External OutMigration</t>
@@ -481,9 +481,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -537,6 +537,38 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Arial"/>
@@ -544,8 +576,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -559,6 +592,64 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -568,53 +659,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -625,51 +670,6 @@
       <color theme="1"/>
       <name val="Arial"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -693,43 +693,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -741,13 +831,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -759,121 +873,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -890,8 +890,23 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -920,21 +935,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -946,15 +946,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -976,6 +967,15 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -987,142 +987,142 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1486,7 +1486,7 @@
   <sheetPr/>
   <dimension ref="A1:O29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
@@ -2412,8 +2412,8 @@
   <sheetPr/>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelRow="1" outlineLevelCol="2"/>

</xml_diff>

<commit_message>
- Add columnCide to CoreFormColumnOptions as part of the support for all Core Form options customization - Add check for data not uploaded on SyncDownloadPanelFragment to avoid sync on all fragments
</commit_message>
<xml_diff>
--- a/app/src/main/res/raw/outmigration_form.xlsx
+++ b/app/src/main/res/raw/outmigration_form.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19485" windowHeight="7560" tabRatio="500" activeTab="1"/>
+    <workbookView windowWidth="18195" windowHeight="9375" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="columns" sheetId="1" r:id="rId1"/>
@@ -475,7 +475,7 @@
     <t>Émigration externe</t>
   </si>
   <si>
-    <t>CAME_WITH_RELATIVES</t>
+    <t>WENT_WITH_RELATIVES</t>
   </si>
   <si>
     <t>Went with relative(s)</t>
@@ -612,10 +612,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="179" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="27">
     <font>
@@ -672,10 +672,26 @@
     </font>
     <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF800080"/>
       <name val="Arial"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -687,10 +703,17 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Arial"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -701,8 +724,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -723,16 +755,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -740,39 +764,15 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -793,7 +793,7 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Arial"/>
       <charset val="134"/>
@@ -832,181 +832,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1097,50 +1097,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1162,11 +1123,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1188,148 +1147,189 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="27" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1342,7 +1342,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1364,10 +1364,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1724,7 +1727,7 @@
   <dimension ref="A1:Q32"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="12.75"/>
@@ -1773,7 +1776,7 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="23" t="s">
+      <c r="J1" s="24" t="s">
         <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
@@ -1788,7 +1791,7 @@
       <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="29" t="s">
+      <c r="O1" s="30" t="s">
         <v>14</v>
       </c>
       <c r="P1" s="1" t="s">
@@ -1804,15 +1807,15 @@
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="E2" s="19" t="s">
         <v>19</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
-      <c r="H2" s="18" t="s">
+      <c r="H2" s="19" t="s">
         <v>20</v>
       </c>
       <c r="I2" t="s">
@@ -1829,7 +1832,7 @@
       <c r="N2" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="O2" s="29"/>
+      <c r="O2" s="30"/>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" s="1" t="s">
@@ -1850,8 +1853,8 @@
       <c r="J3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="K3" s="24"/>
-      <c r="L3" s="24"/>
+      <c r="K3" s="25"/>
+      <c r="L3" s="25"/>
       <c r="M3" t="b">
         <v>1</v>
       </c>
@@ -1876,8 +1879,8 @@
       <c r="J4" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="K4" s="24"/>
-      <c r="L4" s="24"/>
+      <c r="K4" s="25"/>
+      <c r="L4" s="25"/>
       <c r="M4" t="b">
         <v>1</v>
       </c>
@@ -1905,8 +1908,8 @@
       <c r="J5" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="K5" s="24"/>
-      <c r="L5" s="24"/>
+      <c r="K5" s="25"/>
+      <c r="L5" s="25"/>
       <c r="M5" t="b">
         <v>1</v>
       </c>
@@ -1934,8 +1937,8 @@
       <c r="J6" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="K6" s="24"/>
-      <c r="L6" s="24"/>
+      <c r="K6" s="25"/>
+      <c r="L6" s="25"/>
       <c r="M6" t="b">
         <v>1</v>
       </c>
@@ -1960,8 +1963,8 @@
       <c r="J7" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="K7" s="24"/>
-      <c r="L7" s="24"/>
+      <c r="K7" s="25"/>
+      <c r="L7" s="25"/>
       <c r="M7" t="b">
         <v>1</v>
       </c>
@@ -1989,8 +1992,8 @@
       <c r="J8" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="K8" s="24"/>
-      <c r="L8" s="24"/>
+      <c r="K8" s="25"/>
+      <c r="L8" s="25"/>
       <c r="M8" t="b">
         <v>1</v>
       </c>
@@ -2015,8 +2018,8 @@
       <c r="J9" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="K9" s="24"/>
-      <c r="L9" s="24"/>
+      <c r="K9" s="25"/>
+      <c r="L9" s="25"/>
       <c r="M9" t="b">
         <v>1</v>
       </c>
@@ -2041,8 +2044,8 @@
       <c r="J10" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="K10" s="24"/>
-      <c r="L10" s="24"/>
+      <c r="K10" s="25"/>
+      <c r="L10" s="25"/>
       <c r="M10" t="b">
         <v>1</v>
       </c>
@@ -2061,11 +2064,11 @@
       <c r="I11" t="s">
         <v>64</v>
       </c>
-      <c r="J11" s="25" t="s">
+      <c r="J11" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="K11" s="24"/>
-      <c r="L11" s="24"/>
+      <c r="K11" s="25"/>
+      <c r="L11" s="25"/>
       <c r="M11" t="b">
         <v>1</v>
       </c>
@@ -2073,195 +2076,195 @@
         <v>66</v>
       </c>
     </row>
-    <row r="12" s="15" customFormat="1" spans="1:14">
-      <c r="A12" s="19" t="s">
+    <row r="12" s="16" customFormat="1" spans="1:14">
+      <c r="A12" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="D12" s="15" t="s">
+      <c r="D12" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="E12" s="15" t="s">
+      <c r="E12" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="F12" s="22"/>
-      <c r="G12" s="22"/>
-      <c r="H12" s="15" t="s">
+      <c r="F12" s="23"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="I12" s="15" t="s">
+      <c r="I12" s="16" t="s">
         <v>71</v>
       </c>
       <c r="J12" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="K12" s="26"/>
-      <c r="L12" s="26"/>
-      <c r="M12" s="15" t="b">
+      <c r="K12" s="27"/>
+      <c r="L12" s="27"/>
+      <c r="M12" s="16" t="b">
         <v>1</v>
       </c>
-      <c r="N12" s="15" t="b">
+      <c r="N12" s="16" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="13" s="16" customFormat="1" spans="1:14">
-      <c r="A13" s="20" t="s">
+    <row r="13" s="17" customFormat="1" spans="1:14">
+      <c r="A13" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="E13" s="16" t="s">
+      <c r="E13" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="H13" s="16" t="s">
+      <c r="H13" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="I13" s="16" t="s">
+      <c r="I13" s="17" t="s">
         <v>76</v>
       </c>
       <c r="J13" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="K13" s="27"/>
-      <c r="L13" s="27"/>
-      <c r="M13" s="16" t="b">
+      <c r="K13" s="28"/>
+      <c r="L13" s="28"/>
+      <c r="M13" s="17" t="b">
         <v>1</v>
       </c>
-      <c r="N13" s="16" t="b">
+      <c r="N13" s="17" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="14" s="16" customFormat="1" spans="1:17">
-      <c r="A14" s="20" t="s">
+    <row r="14" s="17" customFormat="1" spans="1:17">
+      <c r="A14" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="D14" s="16" t="s">
+      <c r="D14" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="E14" s="16" t="s">
+      <c r="E14" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="H14" s="16" t="s">
+      <c r="H14" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="I14" s="16" t="s">
+      <c r="I14" s="17" t="s">
         <v>80</v>
       </c>
       <c r="J14" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="K14" s="27"/>
-      <c r="L14" s="27"/>
-      <c r="N14" s="16" t="b">
+      <c r="K14" s="28"/>
+      <c r="L14" s="28"/>
+      <c r="N14" s="17" t="b">
         <v>1</v>
       </c>
-      <c r="Q14" s="16" t="b">
+      <c r="Q14" s="17" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="15" s="16" customFormat="1" spans="1:17">
-      <c r="A15" s="20" t="s">
+    <row r="15" s="17" customFormat="1" spans="1:17">
+      <c r="A15" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="D15" s="16" t="s">
+      <c r="D15" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="E15" s="16" t="s">
+      <c r="E15" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="H15" s="16" t="s">
+      <c r="H15" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="I15" s="16" t="s">
+      <c r="I15" s="17" t="s">
         <v>82</v>
       </c>
       <c r="J15" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="K15" s="27"/>
-      <c r="L15" s="27"/>
-      <c r="N15" s="16" t="b">
+      <c r="K15" s="28"/>
+      <c r="L15" s="28"/>
+      <c r="N15" s="17" t="b">
         <v>1</v>
       </c>
-      <c r="Q15" s="16" t="b">
+      <c r="Q15" s="17" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="16" s="16" customFormat="1" spans="1:17">
-      <c r="A16" s="20" t="s">
+    <row r="16" s="17" customFormat="1" spans="1:17">
+      <c r="A16" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="D16" s="16" t="s">
+      <c r="D16" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="E16" s="16" t="s">
+      <c r="E16" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="H16" s="16" t="s">
+      <c r="H16" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="I16" s="16" t="s">
+      <c r="I16" s="17" t="s">
         <v>84</v>
       </c>
       <c r="J16" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="K16" s="27"/>
-      <c r="L16" s="27"/>
-      <c r="N16" s="16" t="b">
+      <c r="K16" s="28"/>
+      <c r="L16" s="28"/>
+      <c r="N16" s="17" t="b">
         <v>1</v>
       </c>
-      <c r="Q16" s="16" t="b">
+      <c r="Q16" s="17" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="17" s="17" customFormat="1" spans="1:14">
-      <c r="A17" s="21" t="s">
+    <row r="17" s="18" customFormat="1" spans="1:14">
+      <c r="A17" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="D17" s="17" t="s">
+      <c r="D17" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="E17" s="17" t="s">
+      <c r="E17" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="H17" s="17" t="s">
+      <c r="H17" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="I17" s="17" t="s">
+      <c r="I17" s="18" t="s">
         <v>87</v>
       </c>
       <c r="J17" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="K17" s="28"/>
-      <c r="L17" s="28"/>
-      <c r="M17" s="17" t="b">
+      <c r="K17" s="29"/>
+      <c r="L17" s="29"/>
+      <c r="M17" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="N17" s="17" t="b">
+      <c r="N17" s="18" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:12">
       <c r="A18" s="1"/>
-      <c r="K18" s="24"/>
-      <c r="L18" s="24"/>
+      <c r="K18" s="25"/>
+      <c r="L18" s="25"/>
     </row>
     <row r="19" spans="1:12">
       <c r="A19" s="1"/>
-      <c r="K19" s="24"/>
-      <c r="L19" s="24"/>
+      <c r="K19" s="25"/>
+      <c r="L19" s="25"/>
     </row>
     <row r="20" spans="1:12">
       <c r="A20" s="1"/>
-      <c r="K20" s="24"/>
-      <c r="L20" s="24"/>
+      <c r="K20" s="25"/>
+      <c r="L20" s="25"/>
     </row>
     <row r="21" spans="1:12">
       <c r="A21" s="1"/>
-      <c r="K21" s="24"/>
-      <c r="L21" s="24"/>
+      <c r="K21" s="25"/>
+      <c r="L21" s="25"/>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" s="1"/>
@@ -2309,7 +2312,7 @@
   <dimension ref="A1:F45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.18095238095238" defaultRowHeight="12.75" outlineLevelCol="5"/>
@@ -2354,7 +2357,7 @@
       <c r="D2" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="13" t="s">
         <v>94</v>
       </c>
       <c r="F2" s="3"/>
@@ -2372,7 +2375,7 @@
       <c r="D3" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="13" t="s">
         <v>98</v>
       </c>
       <c r="F3" s="3"/>
@@ -2390,10 +2393,10 @@
       <c r="D4" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="F4" s="14" t="s">
         <v>104</v>
       </c>
     </row>
@@ -2410,7 +2413,7 @@
       <c r="D5" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="15" t="s">
         <v>108</v>
       </c>
     </row>
@@ -2427,7 +2430,7 @@
       <c r="D6" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="15" t="s">
         <v>112</v>
       </c>
     </row>
@@ -2444,7 +2447,7 @@
       <c r="D7" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="15" t="s">
         <v>116</v>
       </c>
     </row>
@@ -2461,7 +2464,7 @@
       <c r="D8" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E8" s="15" t="s">
         <v>120</v>
       </c>
     </row>
@@ -2478,7 +2481,7 @@
       <c r="D9" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="E9" s="15" t="s">
         <v>124</v>
       </c>
     </row>
@@ -2495,7 +2498,7 @@
       <c r="D10" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="E10" s="15" t="s">
         <v>128</v>
       </c>
     </row>
@@ -2512,7 +2515,7 @@
       <c r="D11" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="E11" s="14" t="s">
+      <c r="E11" s="15" t="s">
         <v>132</v>
       </c>
     </row>
@@ -2529,7 +2532,7 @@
       <c r="D12" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="E12" s="14" t="s">
+      <c r="E12" s="15" t="s">
         <v>136</v>
       </c>
     </row>
@@ -2571,7 +2574,7 @@
       <c r="A15" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="11" t="s">
         <v>145</v>
       </c>
       <c r="C15" s="10" t="s">
@@ -2588,7 +2591,7 @@
       <c r="A16" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="11" t="s">
         <v>149</v>
       </c>
       <c r="C16" s="10" t="s">
@@ -2605,10 +2608,10 @@
       <c r="A17" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C17" s="11" t="s">
         <v>154</v>
       </c>
       <c r="D17" t="s">
@@ -2622,7 +2625,7 @@
       <c r="A18" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="11" t="s">
         <v>157</v>
       </c>
       <c r="C18" s="10" t="s">
@@ -2639,7 +2642,7 @@
       <c r="A19" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="11" t="s">
         <v>161</v>
       </c>
       <c r="C19" s="10" t="s">
@@ -2656,7 +2659,7 @@
       <c r="A20" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="11" t="s">
         <v>165</v>
       </c>
       <c r="C20" s="10" t="s">
@@ -2673,7 +2676,7 @@
       <c r="A21" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="11" t="s">
         <v>169</v>
       </c>
       <c r="C21" s="10" t="s">
@@ -2690,10 +2693,10 @@
       <c r="A22" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="11" t="s">
         <v>173</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C22" s="11" t="s">
         <v>174</v>
       </c>
       <c r="D22" t="s">
@@ -2724,7 +2727,7 @@
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="8"/>
-      <c r="B24" s="11"/>
+      <c r="B24" s="12"/>
       <c r="C24" s="10"/>
       <c r="D24" s="10"/>
       <c r="E24" s="10"/>
@@ -2732,15 +2735,15 @@
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="8"/>
-      <c r="B25" s="11"/>
+      <c r="B25" s="12"/>
       <c r="C25" s="10"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="8"/>
-      <c r="B26" s="11"/>
+      <c r="B26" s="12"/>
       <c r="C26" s="10"/>
       <c r="D26" s="10"/>
       <c r="E26" s="10"/>
@@ -2748,7 +2751,7 @@
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="8"/>
-      <c r="B27" s="11"/>
+      <c r="B27" s="12"/>
       <c r="C27" s="10"/>
       <c r="D27" s="10"/>
       <c r="E27" s="10"/>
@@ -2756,7 +2759,7 @@
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="8"/>
-      <c r="B28" s="11"/>
+      <c r="B28" s="12"/>
       <c r="C28" s="10"/>
       <c r="D28" s="10"/>
       <c r="E28" s="10"/>
@@ -2764,15 +2767,15 @@
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="8"/>
-      <c r="B29" s="11"/>
+      <c r="B29" s="12"/>
       <c r="C29" s="10"/>
       <c r="D29" s="10"/>
       <c r="E29" s="10"/>
-      <c r="F29" s="9"/>
+      <c r="F29" s="11"/>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="8"/>
-      <c r="B30" s="11"/>
+      <c r="B30" s="12"/>
       <c r="C30" s="10"/>
       <c r="D30" s="10"/>
       <c r="E30" s="10"/>
@@ -2780,7 +2783,7 @@
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="8"/>
-      <c r="B31" s="11"/>
+      <c r="B31" s="12"/>
       <c r="C31" s="10"/>
       <c r="D31" s="10"/>
       <c r="E31" s="10"/>
@@ -2788,7 +2791,7 @@
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="8"/>
-      <c r="B32" s="11"/>
+      <c r="B32" s="12"/>
       <c r="C32" s="10"/>
       <c r="D32" s="10"/>
       <c r="E32" s="10"/>
@@ -2796,7 +2799,7 @@
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="8"/>
-      <c r="B33" s="11"/>
+      <c r="B33" s="12"/>
       <c r="C33" s="10"/>
       <c r="D33" s="10"/>
       <c r="E33" s="10"/>
@@ -2804,7 +2807,7 @@
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="8"/>
-      <c r="B34" s="11"/>
+      <c r="B34" s="12"/>
       <c r="C34" s="10"/>
       <c r="D34" s="10"/>
       <c r="E34" s="10"/>
@@ -2812,7 +2815,7 @@
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="8"/>
-      <c r="B35" s="11"/>
+      <c r="B35" s="12"/>
       <c r="C35" s="10"/>
       <c r="D35" s="10"/>
       <c r="E35" s="10"/>
@@ -2828,7 +2831,7 @@
       <c r="F39" s="10"/>
     </row>
     <row r="40" spans="6:6">
-      <c r="F40" s="9"/>
+      <c r="F40" s="11"/>
     </row>
     <row r="41" spans="6:6">
       <c r="F41" s="10"/>

</xml_diff>